<commit_message>
added a function to remove duplicates for data import before post request
</commit_message>
<xml_diff>
--- a/public/sample/excel_1.xlsx
+++ b/public/sample/excel_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="163">
   <si>
     <t>first name</t>
   </si>
@@ -151,364 +151,349 @@
     <t>Scott</t>
   </si>
   <si>
-    <t>alice@example.com</t>
-  </si>
-  <si>
-    <t>bob@example.com</t>
-  </si>
-  <si>
-    <t>carol@example.com</t>
-  </si>
-  <si>
-    <t>dave@example.com</t>
-  </si>
-  <si>
-    <t>eve@example.com</t>
-  </si>
-  <si>
-    <t>frank@example.com</t>
-  </si>
-  <si>
-    <t>grace@example.com</t>
-  </si>
-  <si>
-    <t>heidi@example.com</t>
-  </si>
-  <si>
-    <t>ivan@example.com</t>
-  </si>
-  <si>
-    <t>judy@example.com</t>
-  </si>
-  <si>
-    <t>user011@example.com</t>
-  </si>
-  <si>
-    <t>user012@example.com</t>
-  </si>
-  <si>
-    <t>user013@example.com</t>
-  </si>
-  <si>
-    <t>user014@example.com</t>
-  </si>
-  <si>
-    <t>user015@example.com</t>
-  </si>
-  <si>
-    <t>user016@example.com</t>
-  </si>
-  <si>
-    <t>user017@example.com</t>
-  </si>
-  <si>
-    <t>user018@example.com</t>
-  </si>
-  <si>
-    <t>user019@example.com</t>
-  </si>
-  <si>
-    <t>user020@example.com</t>
-  </si>
-  <si>
-    <t>user021@example.com</t>
-  </si>
-  <si>
-    <t>user022@example.com</t>
-  </si>
-  <si>
-    <t>user023@example.com</t>
-  </si>
-  <si>
-    <t>user024@example.com</t>
-  </si>
-  <si>
-    <t>user025@example.com</t>
-  </si>
-  <si>
-    <t>user026@example.com</t>
-  </si>
-  <si>
-    <t>user027@example.com</t>
-  </si>
-  <si>
-    <t>user028@example.com</t>
-  </si>
-  <si>
-    <t>user029@example.com</t>
-  </si>
-  <si>
-    <t>user030@example.com</t>
-  </si>
-  <si>
-    <t>user031@example.com</t>
-  </si>
-  <si>
-    <t>user032@example.com</t>
-  </si>
-  <si>
-    <t>user033@example.com</t>
-  </si>
-  <si>
-    <t>user034@example.com</t>
-  </si>
-  <si>
-    <t>user035@example.com</t>
-  </si>
-  <si>
-    <t>user036@example.com</t>
-  </si>
-  <si>
-    <t>user037@example.com</t>
-  </si>
-  <si>
-    <t>user038@example.com</t>
-  </si>
-  <si>
-    <t>user039@example.com</t>
-  </si>
-  <si>
-    <t>user040@example.com</t>
-  </si>
-  <si>
-    <t>user041@example.com</t>
-  </si>
-  <si>
-    <t>user042@example.com</t>
-  </si>
-  <si>
-    <t>user043@example.com</t>
-  </si>
-  <si>
-    <t>user044@example.com</t>
-  </si>
-  <si>
-    <t>user045@example.com</t>
-  </si>
-  <si>
-    <t>user046@example.com</t>
-  </si>
-  <si>
-    <t>user047@example.com</t>
-  </si>
-  <si>
-    <t>user048@example.com</t>
-  </si>
-  <si>
-    <t>user049@example.com</t>
-  </si>
-  <si>
-    <t>user050@example.com</t>
-  </si>
-  <si>
-    <t>user051@example.com</t>
-  </si>
-  <si>
-    <t>user052@example.com</t>
-  </si>
-  <si>
-    <t>user053@example.com</t>
-  </si>
-  <si>
-    <t>user054@example.com</t>
-  </si>
-  <si>
-    <t>user055@example.com</t>
-  </si>
-  <si>
-    <t>user056@example.com</t>
-  </si>
-  <si>
-    <t>user057@example.com</t>
-  </si>
-  <si>
-    <t>user058@example.com</t>
-  </si>
-  <si>
-    <t>user059@example.com</t>
-  </si>
-  <si>
-    <t>user060@example.com</t>
-  </si>
-  <si>
-    <t>CS001</t>
-  </si>
-  <si>
-    <t>DSI002</t>
-  </si>
-  <si>
-    <t>IT003</t>
-  </si>
-  <si>
-    <t>CS004</t>
-  </si>
-  <si>
-    <t>DSI005</t>
-  </si>
-  <si>
-    <t>IT006</t>
-  </si>
-  <si>
-    <t>CS007</t>
-  </si>
-  <si>
-    <t>DSI008</t>
-  </si>
-  <si>
-    <t>IT009</t>
-  </si>
-  <si>
-    <t>CS010</t>
-  </si>
-  <si>
-    <t>CS011</t>
-  </si>
-  <si>
-    <t>IT012</t>
-  </si>
-  <si>
-    <t>CS013</t>
-  </si>
-  <si>
-    <t>DSI014</t>
-  </si>
-  <si>
-    <t>DSI015</t>
-  </si>
-  <si>
-    <t>IT016</t>
-  </si>
-  <si>
-    <t>CS017</t>
-  </si>
-  <si>
-    <t>CS018</t>
-  </si>
-  <si>
-    <t>CS019</t>
-  </si>
-  <si>
-    <t>CS020</t>
-  </si>
-  <si>
-    <t>IT021</t>
-  </si>
-  <si>
-    <t>CS022</t>
-  </si>
-  <si>
-    <t>DSI023</t>
-  </si>
-  <si>
-    <t>IT024</t>
-  </si>
-  <si>
-    <t>IT025</t>
-  </si>
-  <si>
-    <t>CS026</t>
-  </si>
-  <si>
-    <t>DSI027</t>
-  </si>
-  <si>
-    <t>CS028</t>
-  </si>
-  <si>
-    <t>DSI029</t>
-  </si>
-  <si>
-    <t>CS030</t>
-  </si>
-  <si>
-    <t>IT031</t>
-  </si>
-  <si>
-    <t>DSI032</t>
-  </si>
-  <si>
-    <t>DSI033</t>
-  </si>
-  <si>
-    <t>DSI034</t>
-  </si>
-  <si>
-    <t>CS035</t>
-  </si>
-  <si>
-    <t>IT036</t>
-  </si>
-  <si>
-    <t>IT037</t>
-  </si>
-  <si>
-    <t>CS038</t>
-  </si>
-  <si>
-    <t>CS039</t>
-  </si>
-  <si>
-    <t>IT040</t>
-  </si>
-  <si>
-    <t>CS041</t>
-  </si>
-  <si>
-    <t>IT042</t>
-  </si>
-  <si>
-    <t>IT043</t>
-  </si>
-  <si>
-    <t>CS044</t>
-  </si>
-  <si>
-    <t>IT045</t>
-  </si>
-  <si>
-    <t>IT046</t>
-  </si>
-  <si>
-    <t>CS047</t>
-  </si>
-  <si>
-    <t>IT048</t>
-  </si>
-  <si>
-    <t>CS049</t>
-  </si>
-  <si>
-    <t>DSI050</t>
-  </si>
-  <si>
-    <t>CS051</t>
-  </si>
-  <si>
-    <t>DSI052</t>
-  </si>
-  <si>
-    <t>IT053</t>
-  </si>
-  <si>
-    <t>IT054</t>
-  </si>
-  <si>
-    <t>CS055</t>
-  </si>
-  <si>
-    <t>IT056</t>
-  </si>
-  <si>
-    <t>CS057</t>
-  </si>
-  <si>
-    <t>DSI058</t>
-  </si>
-  <si>
-    <t>IT059</t>
-  </si>
-  <si>
-    <t>CS060</t>
+    <t>harley.turner@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>blake.brown@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>jules.davis@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>nico.brown@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>parker.nguyen@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>sage.lee@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>dana.turner@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>parker.garcia@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>quinn.anderson@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>kai.young@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>alex.lee@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>blake.davis@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>oakley.zimmerman@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>alex.walker@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>logan.robinson@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>oakley.johnson@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>dana.walker@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>dana.nguyen@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>indie.patel@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>casey.brown@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>morgan.garcia@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>morgan.walker@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>dana.davis@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>parker.anderson@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>georgie.robinson@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>parker.walker@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>dana.evans@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>indie.evans@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>harley.patel@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>alex.turner@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>parker.brown@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>oakley.evans@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>kai.clark@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>emery.harris@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>riley.young@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>riley.zimmerman@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>finn.patel@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>morgan.zimmerman@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>riley.nguyen@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>blake.robinson@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>georgie.smith@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>nico.walker@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>blake.martinez@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>jules.nguyen@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>kai.lee@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>alex.smith@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>sage.young@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>kai.brown@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>oakley.patel@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>parker.clark@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>sage.smith@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>logan.harris@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>harley.lee@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>finn.brown@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>jamie.scott@ad.sit.kmutt.ac.th</t>
+  </si>
+  <si>
+    <t>74352229315</t>
+  </si>
+  <si>
+    <t>21780329309</t>
+  </si>
+  <si>
+    <t>35002758059</t>
+  </si>
+  <si>
+    <t>99227597028</t>
+  </si>
+  <si>
+    <t>33528768742</t>
+  </si>
+  <si>
+    <t>89672459697</t>
+  </si>
+  <si>
+    <t>21481115909</t>
+  </si>
+  <si>
+    <t>97621460892</t>
+  </si>
+  <si>
+    <t>75614942826</t>
+  </si>
+  <si>
+    <t>41889397930</t>
+  </si>
+  <si>
+    <t>75954479752</t>
+  </si>
+  <si>
+    <t>58201693518</t>
+  </si>
+  <si>
+    <t>57739771776</t>
+  </si>
+  <si>
+    <t>67400395657</t>
+  </si>
+  <si>
+    <t>40230613092</t>
+  </si>
+  <si>
+    <t>34760431574</t>
+  </si>
+  <si>
+    <t>86994896418</t>
+  </si>
+  <si>
+    <t>45388500411</t>
+  </si>
+  <si>
+    <t>36952123614</t>
+  </si>
+  <si>
+    <t>37237172863</t>
+  </si>
+  <si>
+    <t>39864441273</t>
+  </si>
+  <si>
+    <t>39394135318</t>
+  </si>
+  <si>
+    <t>14226991079</t>
+  </si>
+  <si>
+    <t>18384655591</t>
+  </si>
+  <si>
+    <t>88845793218</t>
+  </si>
+  <si>
+    <t>80148493427</t>
+  </si>
+  <si>
+    <t>56649628891</t>
+  </si>
+  <si>
+    <t>36058985129</t>
+  </si>
+  <si>
+    <t>63235395640</t>
+  </si>
+  <si>
+    <t>22147223708</t>
+  </si>
+  <si>
+    <t>71517148044</t>
+  </si>
+  <si>
+    <t>32075328123</t>
+  </si>
+  <si>
+    <t>88255444222</t>
+  </si>
+  <si>
+    <t>87075252638</t>
+  </si>
+  <si>
+    <t>78846582354</t>
+  </si>
+  <si>
+    <t>11618711516</t>
+  </si>
+  <si>
+    <t>73438262397</t>
+  </si>
+  <si>
+    <t>48704951412</t>
+  </si>
+  <si>
+    <t>83124221192</t>
+  </si>
+  <si>
+    <t>55424674095</t>
+  </si>
+  <si>
+    <t>15921957837</t>
+  </si>
+  <si>
+    <t>45500368093</t>
+  </si>
+  <si>
+    <t>90799804216</t>
+  </si>
+  <si>
+    <t>77862534364</t>
+  </si>
+  <si>
+    <t>54369621988</t>
+  </si>
+  <si>
+    <t>63024490354</t>
+  </si>
+  <si>
+    <t>81354932218</t>
+  </si>
+  <si>
+    <t>48179048195</t>
+  </si>
+  <si>
+    <t>66495372826</t>
+  </si>
+  <si>
+    <t>80292768857</t>
+  </si>
+  <si>
+    <t>46760544652</t>
+  </si>
+  <si>
+    <t>37191506025</t>
+  </si>
+  <si>
+    <t>18319477036</t>
+  </si>
+  <si>
+    <t>66347251744</t>
+  </si>
+  <si>
+    <t>67356081917</t>
+  </si>
+  <si>
+    <t>83172039407</t>
+  </si>
+  <si>
+    <t>60658951650</t>
+  </si>
+  <si>
+    <t>12575476999</t>
+  </si>
+  <si>
+    <t>10048441739</t>
+  </si>
+  <si>
+    <t>30626357399</t>
   </si>
   <si>
     <t>CS</t>
@@ -518,12 +503,6 @@
   </si>
   <si>
     <t>IT</t>
-  </si>
-  <si>
-    <t>2024-2025</t>
-  </si>
-  <si>
-    <t>2025-2026</t>
   </si>
 </sst>
 </file>
@@ -918,13 +897,13 @@
         <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
-      </c>
-      <c r="F2" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="F2">
+        <v>2024</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -938,13 +917,13 @@
         <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F3" t="s">
-        <v>168</v>
+        <v>161</v>
+      </c>
+      <c r="F3">
+        <v>2025</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -958,13 +937,13 @@
         <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>167</v>
-      </c>
-      <c r="F4" t="s">
-        <v>169</v>
+        <v>162</v>
+      </c>
+      <c r="F4">
+        <v>2024</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -978,13 +957,13 @@
         <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F5" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="F5">
+        <v>2025</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -998,13 +977,13 @@
         <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E6" t="s">
-        <v>166</v>
-      </c>
-      <c r="F6" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F6">
+        <v>2024</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1015,16 +994,16 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E7" t="s">
-        <v>167</v>
-      </c>
-      <c r="F7" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="F7">
+        <v>2025</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1035,16 +1014,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>165</v>
-      </c>
-      <c r="F8" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="F8">
+        <v>2024</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1055,16 +1034,16 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
-      </c>
-      <c r="F9" t="s">
-        <v>168</v>
+        <v>161</v>
+      </c>
+      <c r="F9">
+        <v>2025</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1075,16 +1054,16 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E10" t="s">
-        <v>167</v>
-      </c>
-      <c r="F10" t="s">
-        <v>169</v>
+        <v>162</v>
+      </c>
+      <c r="F10">
+        <v>2024</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1095,16 +1074,16 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E11" t="s">
-        <v>165</v>
-      </c>
-      <c r="F11" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="F11">
+        <v>2025</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1115,16 +1094,16 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E12" t="s">
-        <v>165</v>
-      </c>
-      <c r="F12" t="s">
-        <v>168</v>
+        <v>161</v>
+      </c>
+      <c r="F12">
+        <v>2024</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1135,16 +1114,16 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E13" t="s">
-        <v>167</v>
-      </c>
-      <c r="F13" t="s">
-        <v>169</v>
+        <v>162</v>
+      </c>
+      <c r="F13">
+        <v>2025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1155,16 +1134,16 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E14" t="s">
-        <v>165</v>
-      </c>
-      <c r="F14" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="F14">
+        <v>2024</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1175,16 +1154,16 @@
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E15" t="s">
-        <v>166</v>
-      </c>
-      <c r="F15" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F15">
+        <v>2025</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1195,16 +1174,16 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E16" t="s">
-        <v>166</v>
-      </c>
-      <c r="F16" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="F16">
+        <v>2024</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1215,16 +1194,16 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E17" t="s">
-        <v>167</v>
-      </c>
-      <c r="F17" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="F17">
+        <v>2025</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1235,16 +1214,16 @@
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F18" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F18">
+        <v>2024</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1255,16 +1234,16 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E19" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" t="s">
-        <v>169</v>
+        <v>162</v>
+      </c>
+      <c r="F19">
+        <v>2025</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1275,16 +1254,16 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E20" t="s">
-        <v>165</v>
-      </c>
-      <c r="F20" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="F20">
+        <v>2024</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1295,16 +1274,16 @@
         <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E21" t="s">
-        <v>165</v>
-      </c>
-      <c r="F21" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F21">
+        <v>2025</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1315,16 +1294,16 @@
         <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E22" t="s">
-        <v>167</v>
-      </c>
-      <c r="F22" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="F22">
+        <v>2024</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1335,16 +1314,16 @@
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E23" t="s">
-        <v>165</v>
-      </c>
-      <c r="F23" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="F23">
+        <v>2025</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1355,16 +1334,16 @@
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E24" t="s">
-        <v>166</v>
-      </c>
-      <c r="F24" t="s">
-        <v>168</v>
+        <v>161</v>
+      </c>
+      <c r="F24">
+        <v>2024</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1375,16 +1354,16 @@
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E25" t="s">
-        <v>167</v>
-      </c>
-      <c r="F25" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="F25">
+        <v>2025</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1395,16 +1374,16 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E26" t="s">
-        <v>167</v>
-      </c>
-      <c r="F26" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="F26">
+        <v>2024</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1415,16 +1394,16 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E27" t="s">
-        <v>165</v>
-      </c>
-      <c r="F27" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F27">
+        <v>2025</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1435,16 +1414,16 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E28" t="s">
-        <v>166</v>
-      </c>
-      <c r="F28" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="F28">
+        <v>2024</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1455,16 +1434,16 @@
         <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E29" t="s">
-        <v>165</v>
-      </c>
-      <c r="F29" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="F29">
+        <v>2025</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1475,16 +1454,16 @@
         <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E30" t="s">
-        <v>166</v>
-      </c>
-      <c r="F30" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F30">
+        <v>2024</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1495,16 +1474,16 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D31" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E31" t="s">
-        <v>165</v>
-      </c>
-      <c r="F31" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="F31">
+        <v>2025</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1515,16 +1494,16 @@
         <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D32" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E32" t="s">
-        <v>167</v>
-      </c>
-      <c r="F32" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="F32">
+        <v>2024</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1535,16 +1514,16 @@
         <v>26</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D33" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E33" t="s">
-        <v>166</v>
-      </c>
-      <c r="F33" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F33">
+        <v>2025</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1555,16 +1534,16 @@
         <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E34" t="s">
-        <v>166</v>
-      </c>
-      <c r="F34" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="F34">
+        <v>2024</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1575,16 +1554,16 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E35" t="s">
-        <v>166</v>
-      </c>
-      <c r="F35" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="F35">
+        <v>2025</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1595,16 +1574,16 @@
         <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E36" t="s">
-        <v>165</v>
-      </c>
-      <c r="F36" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F36">
+        <v>2024</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1615,16 +1594,16 @@
         <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D37" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E37" t="s">
-        <v>167</v>
-      </c>
-      <c r="F37" t="s">
-        <v>169</v>
+        <v>162</v>
+      </c>
+      <c r="F37">
+        <v>2025</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1635,16 +1614,16 @@
         <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D38" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E38" t="s">
-        <v>167</v>
-      </c>
-      <c r="F38" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="F38">
+        <v>2024</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1655,16 +1634,16 @@
         <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E39" t="s">
-        <v>165</v>
-      </c>
-      <c r="F39" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F39">
+        <v>2025</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1675,16 +1654,16 @@
         <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D40" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E40" t="s">
-        <v>165</v>
-      </c>
-      <c r="F40" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="F40">
+        <v>2024</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1695,16 +1674,16 @@
         <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D41" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E41" t="s">
-        <v>167</v>
-      </c>
-      <c r="F41" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="F41">
+        <v>2025</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1715,16 +1694,16 @@
         <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D42" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E42" t="s">
-        <v>165</v>
-      </c>
-      <c r="F42" t="s">
-        <v>168</v>
+        <v>161</v>
+      </c>
+      <c r="F42">
+        <v>2024</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1735,16 +1714,16 @@
         <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D43" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E43" t="s">
-        <v>167</v>
-      </c>
-      <c r="F43" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="F43">
+        <v>2025</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1755,16 +1734,16 @@
         <v>36</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D44" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E44" t="s">
-        <v>167</v>
-      </c>
-      <c r="F44" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="F44">
+        <v>2024</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1775,16 +1754,16 @@
         <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D45" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E45" t="s">
-        <v>165</v>
-      </c>
-      <c r="F45" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F45">
+        <v>2025</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1795,16 +1774,16 @@
         <v>35</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D46" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E46" t="s">
-        <v>167</v>
-      </c>
-      <c r="F46" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="F46">
+        <v>2024</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1815,16 +1794,16 @@
         <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D47" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E47" t="s">
-        <v>167</v>
-      </c>
-      <c r="F47" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="F47">
+        <v>2025</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1835,16 +1814,16 @@
         <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D48" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E48" t="s">
-        <v>165</v>
-      </c>
-      <c r="F48" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F48">
+        <v>2024</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1855,16 +1834,16 @@
         <v>30</v>
       </c>
       <c r="C49" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D49" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E49" t="s">
-        <v>167</v>
-      </c>
-      <c r="F49" t="s">
-        <v>169</v>
+        <v>162</v>
+      </c>
+      <c r="F49">
+        <v>2025</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1875,16 +1854,16 @@
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D50" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E50" t="s">
-        <v>165</v>
-      </c>
-      <c r="F50" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="F50">
+        <v>2024</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1895,16 +1874,16 @@
         <v>33</v>
       </c>
       <c r="C51" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D51" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E51" t="s">
-        <v>166</v>
-      </c>
-      <c r="F51" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F51">
+        <v>2025</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1915,16 +1894,16 @@
         <v>27</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D52" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E52" t="s">
-        <v>165</v>
-      </c>
-      <c r="F52" t="s">
-        <v>169</v>
+        <v>162</v>
+      </c>
+      <c r="F52">
+        <v>2024</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1935,16 +1914,16 @@
         <v>38</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D53" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E53" t="s">
-        <v>166</v>
-      </c>
-      <c r="F53" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="F53">
+        <v>2025</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1955,16 +1934,16 @@
         <v>40</v>
       </c>
       <c r="C54" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D54" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E54" t="s">
-        <v>167</v>
-      </c>
-      <c r="F54" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F54">
+        <v>2024</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1975,16 +1954,16 @@
         <v>28</v>
       </c>
       <c r="C55" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="D55" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E55" t="s">
-        <v>167</v>
-      </c>
-      <c r="F55" t="s">
-        <v>169</v>
+        <v>162</v>
+      </c>
+      <c r="F55">
+        <v>2025</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1995,16 +1974,16 @@
         <v>38</v>
       </c>
       <c r="C56" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="D56" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E56" t="s">
-        <v>165</v>
-      </c>
-      <c r="F56" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="F56">
+        <v>2024</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2015,16 +1994,16 @@
         <v>42</v>
       </c>
       <c r="C57" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D57" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E57" t="s">
-        <v>167</v>
-      </c>
-      <c r="F57" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F57">
+        <v>2025</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2035,16 +2014,16 @@
         <v>41</v>
       </c>
       <c r="C58" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D58" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E58" t="s">
-        <v>165</v>
-      </c>
-      <c r="F58" t="s">
-        <v>169</v>
+        <v>162</v>
+      </c>
+      <c r="F58">
+        <v>2024</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2055,16 +2034,16 @@
         <v>30</v>
       </c>
       <c r="C59" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D59" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E59" t="s">
-        <v>166</v>
-      </c>
-      <c r="F59" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+      <c r="F59">
+        <v>2025</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2075,16 +2054,16 @@
         <v>27</v>
       </c>
       <c r="C60" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D60" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E60" t="s">
-        <v>167</v>
-      </c>
-      <c r="F60" t="s">
-        <v>169</v>
+        <v>161</v>
+      </c>
+      <c r="F60">
+        <v>2024</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2095,16 +2074,16 @@
         <v>44</v>
       </c>
       <c r="C61" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D61" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E61" t="s">
-        <v>165</v>
-      </c>
-      <c r="F61" t="s">
-        <v>169</v>
+        <v>162</v>
+      </c>
+      <c r="F61">
+        <v>2025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>